<commit_message>
Cache mapped CellStyles in SXSSFWriter to prevent Index Matching Errors
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/excel/Formatting.xlsx
+++ b/src/test/resources/templates/excel/Formatting.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander/Code/opensource/libraries/jocument/src/test/resources/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E58AE5-A719-A048-B1FD-4743311D6092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9FFC0A-CEAB-2F46-BA11-377009CBAB63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="2200" windowWidth="27640" windowHeight="16940" xr2:uid="{DA9C1F78-8A22-BA4D-A4AA-866704660E49}"/>
+    <workbookView xWindow="10800" yWindow="7660" windowWidth="27640" windowHeight="16940" xr2:uid="{DA9C1F78-8A22-BA4D-A4AA-866704660E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,16 +34,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>{{this}}</t>
+  </si>
+  <si>
+    <t>{{/this}}</t>
+  </si>
+  <si>
+    <t>{{name}}</t>
+  </si>
   <si>
     <t>Hello, World</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>{{rank}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -59,6 +77,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -68,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,14 +102,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FC1811-A5AB-CE42-8B8E-A11F91E9BF42}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,16 +505,42 @@
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:1" ht="31" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44236</v>
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>